<commit_message>
Novos selects adicionados ao excel.
</commit_message>
<xml_diff>
--- a/cartas_e_matriz_gabarito_game_of_selects.xlsx
+++ b/cartas_e_matriz_gabarito_game_of_selects.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="58">
   <si>
     <t>Conteúdo do Select</t>
   </si>
@@ -253,9 +253,6 @@
     <t>SELECT nome FROM monstros WHERE dano &lt;= 180 AND tipo = 'Apóstolo de Mori';</t>
   </si>
   <si>
-    <t>Mostre todos os territórios que possuem monstros de tipo espírito (os dados NÃO podem se repetir)</t>
-  </si>
-  <si>
     <t xml:space="preserve">SELECT DISTINCT(t.nome) FROM territorios AS t JOIN monstros AS m ON m.fk_territorio = t.id_territorio WHERE m.tipo = 'Espírito'; </t>
   </si>
   <si>
@@ -311,6 +308,27 @@
   </si>
   <si>
     <t>Mostre o nome e o dano da arma mais poderosa.</t>
+  </si>
+  <si>
+    <t>Mostre todos os clãs, seus respectivos personagens e territórios.</t>
+  </si>
+  <si>
+    <t>Mostre todos os territórios que possuem monstros de tipo espírito (os dados não podem se repetir)</t>
+  </si>
+  <si>
+    <t>SELECT c.nome, p.nome, t.nome FROM personagens AS p RIGHT JOIN clas AS c ON p.fk_cla = c.id_cla JOIN territorios AS t ON c.fk_territorio = t.id_territorio;</t>
+  </si>
+  <si>
+    <t>Mostre todos os clãs dos territórios que começam com "Reino".</t>
+  </si>
+  <si>
+    <t>SELECT c.nome FROM clas AS c JOIN territorios AS t ON c.fk_territorio = t.id_territorio WHERE t.nome LIKE 'Reino%';</t>
+  </si>
+  <si>
+    <t>Mostre a idade do personagem mais velho, do mais novo e a média arredondada (uma casa decimal) das idades dos membros do clã Nogueirivitcs.</t>
+  </si>
+  <si>
+    <t>SELECT max(p.idade), min(p.idade), round(AVG(p.idade),1) FROM personagens AS p JOIN clas AS c ON p.fk_cla = c.id_cla WHERE c.nome = 'Nogueirivitcs';</t>
   </si>
 </sst>
 </file>
@@ -387,6 +405,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -899,7 +918,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -909,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,10 +974,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>1</v>
@@ -995,10 +1014,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="32" t="s">
         <v>44</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>45</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>1</v>
@@ -1015,10 +1034,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>47</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>1</v>
@@ -1035,10 +1054,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>1</v>
@@ -1048,18 +1067,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="5">
         <v>6</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>1</v>
@@ -1247,10 +1260,10 @@
         <v>16</v>
       </c>
       <c r="C17" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="18" t="s">
         <v>32</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>33</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>9</v>
@@ -1268,10 +1281,10 @@
         <v>17</v>
       </c>
       <c r="C18" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>34</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>35</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>9</v>
@@ -1289,10 +1302,10 @@
         <v>18</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>9</v>
@@ -1310,10 +1323,10 @@
         <v>19</v>
       </c>
       <c r="C20" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>42</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>43</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>9</v>
@@ -1323,12 +1336,18 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>6</v>
       </c>
       <c r="B21" s="5">
         <v>20</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>9</v>
@@ -1338,7 +1357,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>6</v>
       </c>
@@ -1346,10 +1365,10 @@
         <v>21</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>9</v>
@@ -1359,16 +1378,18 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>6</v>
       </c>
       <c r="B23" s="19">
         <v>22</v>
       </c>
-      <c r="C23" s="27"/>
+      <c r="C23" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="D23" s="10" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>9</v>
@@ -1443,10 +1464,10 @@
         <v>26</v>
       </c>
       <c r="C27" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="18" t="s">
         <v>40</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>41</v>
       </c>
       <c r="E27" s="30" t="s">
         <v>3</v>
@@ -1456,15 +1477,19 @@
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
         <v>6</v>
       </c>
       <c r="B28" s="19">
         <v>27</v>
       </c>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
+      <c r="C28" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="E28" s="19" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Excel concluido, modelagem e script atualizados.
</commit_message>
<xml_diff>
--- a/cartas_e_matriz_gabarito_game_of_selects.xlsx
+++ b/cartas_e_matriz_gabarito_game_of_selects.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25401"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B378F3F-C975-4223-85A3-464E18E93585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="cartas.xlsx" sheetId="1" r:id="rId1"/>
     <sheet name="matriz" sheetId="2" r:id="rId2"/>
     <sheet name="Exemplo de Controle" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="92">
   <si>
     <t>SEU NÚMERO DO GRUPO</t>
   </si>
@@ -204,9 +203,6 @@
     <t>SELECT nome, tem_fragmento FROM territorios WHERE tem_fragmento = 'sim' AND area &gt; 3300;</t>
   </si>
   <si>
-    <t>SELECT</t>
-  </si>
-  <si>
     <t>Mostre todos os territórios que possuem monstros de tipo espírito (os dados não podem se repetir)</t>
   </si>
   <si>
@@ -271,15 +267,6 @@
   </si>
   <si>
     <t>SELECT t.nome, (sum(c.qtd_membros) / t.area) FROM clas AS c JOIN territorios AS t ON c.fk_territorio = t.id_territorio GROUP BY t.nome;</t>
-  </si>
-  <si>
-    <t>etc</t>
-  </si>
-  <si>
-    <t>Mostre os nomes, o total de membros de clã, a quantidade total de personagens, o dano total (de personagens e monstros), a quantidade total de raças diferentes e a pontuação total de vida dos monstros de cada território.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELECT t.nome, sum(c.qtd_membros), count(p.id_personagem), sum(a.dano) + sum(m.dano), count(DISTINCT(r.id_raca), sum(m.vida) FROM </t>
   </si>
   <si>
     <t>Challenge</t>
@@ -344,12 +331,147 @@
   <si>
     <t>Grupo 1234</t>
   </si>
+  <si>
+    <t>Mostre o nome em ordem alfabética, a classe e o apelido dos personagens com a vida superior a 500.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+SELECT  nome, classe , apelido FROM personagens WHERE vida &gt; 500 ORDER BY  nome;</t>
+  </si>
+  <si>
+    <t>Mostre o nome e o tipo dos monstros onde o tipo é diferente de Solari e o dano é superior a 40.</t>
+  </si>
+  <si>
+    <t>SELECT nome, tipo FROM monstros WHERE tipo != 'Solari' AND dano &gt; 40;</t>
+  </si>
+  <si>
+    <t>SELECT nome, grito_guerra FROM clas WHERE qtd_membros &gt;= 600 AND qtd_membros &lt;= 900 AND nome LIKE 'M%' OR nome LIKE 'N%' ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Mostre o nome e o grito de guerra dos clãs onde a quantidade de membros está entre 600 e 900 e a primeira letra do clã seja M ou N.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Mostre o nome das raças que tem resistência a queda ou magia, e das raças que tem fraqueza a armas de impacto.</t>
+  </si>
+  <si>
+    <t>SELECT nome_raca FROM racas WHERE resistencia LIKE '%queda%' OR resistencia LIKE '%magia%' OR fraqueza LIKE '%impacto%';</t>
+  </si>
+  <si>
+    <t>Mostre a média de dano, a somatória da vida, a maior e a menor idade dos personagens homens.</t>
+  </si>
+  <si>
+    <t>SELECT avg(a.dano), sum(p.vida), max(p.idade), min(p.idade) FROM armas AS a JOIN personagens AS p ON p.fk_arma = a.id_arma WHERE p.sexo = 'M';</t>
+  </si>
+  <si>
+    <t>Mostre os territórios que têm mais armas e a quantidade.</t>
+  </si>
+  <si>
+    <t>SELECT t.nome, count(p.fk_cla)
+FROM personagens AS p 
+JOIN armas AS a ON p.fk_arma = a.id_arma 
+JOIN clas AS c ON p.fk_cla = c.id_cla 
+JOIN territorios AS t ON c.fk_territorio = t.id_territorio
+GROUP BY t.id_territorio
+ORDER BY count(fk_cla) DESC
+LIMIT 2;</t>
+  </si>
+  <si>
+    <t>Mostre as armas que não tem ligação com nenhum personagem</t>
+  </si>
+  <si>
+    <t>SELECT a.nome FROM armas AS a
+LEFT JOIN personagens AS p
+ON p.fk_arma = a.id_arma WHERE p.nome IS NULL;</t>
+  </si>
+  <si>
+    <t>Mostre todos os monstros que a segunda letra do 
+nome seja "o" e os pontos de vida sejam menores
+que 500.</t>
+  </si>
+  <si>
+    <t>SELECT * FROM monstros  WHERE nome LIKE "_o%" AND pontos_vida &lt; 500 ;</t>
+  </si>
+  <si>
+    <t>SELECT nome_raca, descricao FROM racas WHERE fraqueza = 'Cansa rápido';</t>
+  </si>
+  <si>
+    <t>Mostre o nome e a descrição das raças que a fraqueza seja "Cansa rápido".</t>
+  </si>
+  <si>
+    <t>Mostre as armas e seus respectivos danos, mostrando do menor dano para o maior</t>
+  </si>
+  <si>
+    <t>SELECT nome, dano FROM armas ORDER BY dano ASC;</t>
+  </si>
+  <si>
+    <t>Mostre o nome, o tipo e o dano dos montros ordenados por dano e por tipo 'chefe' crescente</t>
+  </si>
+  <si>
+    <t>SELECT nome, tipo , dano FROM monstros ORDER BY dano AND tipo = 'chefe' DESC;</t>
+  </si>
+  <si>
+    <t>Mostre os monstros ordenados por maior dano, e a qual territorio ele pertence.</t>
+  </si>
+  <si>
+    <t>SELECT m.nome, m.pontos_vida, t.nome
+FROM monstros AS m
+JOIN territorio AS t
+ON m.fk_territorio = t.id_territorio
+ORDER BY pontos_vida ASC;</t>
+  </si>
+  <si>
+    <t>Mostre o nome e o líder dos territórios que o nome começa com "Reino".</t>
+  </si>
+  <si>
+    <t>SELECT nome, lider FROM territorios WHERE nome LIKE ('Reino%');</t>
+  </si>
+  <si>
+    <t>Mostre o nome e a classe dos personagens onde a vida dividida pela idade é maior que 15</t>
+  </si>
+  <si>
+    <t>SELECT nome, classe FROM personagens WHERE vida / idade &gt; 15;</t>
+  </si>
+  <si>
+    <t>Mostre quantas raças têm como fraqueza algum tipo de magia.</t>
+  </si>
+  <si>
+    <t>SELECT count(fraqueza) FROM racas WHERE fraqueza LIKE "magia%";</t>
+  </si>
+  <si>
+    <t>SELECT p.nome, r.nome_raca, a.nome, a.dano, a.tipo, c.nome, r.fraqueza
+FROM personagens AS p
+JOIN racas AS r ON p.fk_raca = r.id_raca
+JOIN armas AS a ON p.fk_arma = a.id_arma
+JOIN clas AS c ON p.fk_cla = c.id_cla
+WHERE a.dano &gt; 30
+AND r.fraqueza like "magia%"
+AND r.nome_raca = "Demônio"
+ORDER BY a.dano ASC;</t>
+  </si>
+  <si>
+    <t>Mostre os personagens que são da raça demônio, suas armas e seus respectivos danos ordenados do menor dano para o maior e que tenham mais de 30 de dano, o nome do clã ao qual o personagem pertence, e que tenham como fraqueza algum tipo de magia.</t>
+  </si>
+  <si>
+    <t>Mostre o nome dos personagens, todos os dados da sua raça,  todos os dados de sua arma, o nome do clã que ele pertence, o nome do território que ele pertence, o nome dos monstros que ele pode enfrentar em seu território e a pontuação de vida e de dano de cada monstro.</t>
+  </si>
+  <si>
+    <t>SELECT p.nome, r.*, a.*, c.nome, t.nome, m.nome, m.pontos_vida, m.dano
+FROM personagens AS p
+JOIN racas AS r ON p.fk_raca = r.id_raca
+JOIN armas AS a ON p.fk_arma = a.id_arma
+JOIN clas AS c ON p.fk_cla = c.id_cla
+JOIN territorios AS t ON t.id_territorio = c.fk_territorio
+JOIN monstros AS m ON t.id_territorio = m.fk_territorio
+ORDER BY c.nome;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -566,7 +688,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -622,9 +744,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -635,6 +754,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -943,21 +1066,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
@@ -968,7 +1091,7 @@
     <col min="7" max="7" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="90">
+    <row r="1" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -991,7 +1114,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6</v>
       </c>
@@ -1011,7 +1134,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30">
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>6</v>
       </c>
@@ -1031,17 +1154,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18" customHeight="1">
+    <row r="4" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="26" t="s">
         <v>13</v>
       </c>
       <c r="E4" t="s">
@@ -1051,7 +1174,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30">
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
@@ -1071,14 +1194,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30">
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="28" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="9" t="s">
@@ -1091,15 +1214,19 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16.5" customHeight="1">
+    <row r="7" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7"/>
-      <c r="D7"/>
+      <c r="C7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>59</v>
+      </c>
       <c r="E7" t="s">
         <v>9</v>
       </c>
@@ -1107,15 +1234,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
+      <c r="C8" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="D8" s="9" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
@@ -1124,15 +1254,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
+      <c r="C9" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="D9" s="9" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -1140,16 +1273,20 @@
       <c r="G9" s="10">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="K9" s="31"/>
+    </row>
+    <row r="10" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
+      <c r="C10" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="D10" s="9" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -1158,15 +1295,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
+      <c r="C11" s="32" t="s">
+        <v>72</v>
+      </c>
       <c r="D11" s="9" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -1175,15 +1315,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
+      <c r="C12" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="D12" s="9" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
@@ -1192,15 +1335,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
+      <c r="C13" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="D13" s="9" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
@@ -1209,15 +1355,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
+      <c r="C14" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="D14" s="9" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
@@ -1226,15 +1375,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
+      <c r="C15" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="D15" s="9" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="E15" t="s">
         <v>9</v>
@@ -1243,15 +1395,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
+      <c r="C16" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="D16" s="9" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
@@ -1260,7 +1415,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="45">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>6</v>
       </c>
@@ -1268,20 +1423,20 @@
         <v>16</v>
       </c>
       <c r="C17" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="E17" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="7">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1289,19 +1444,19 @@
         <v>17</v>
       </c>
       <c r="C18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="E18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G18" s="10">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="45">
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6</v>
       </c>
@@ -1309,19 +1464,19 @@
         <v>18</v>
       </c>
       <c r="C19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>25</v>
-      </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G19" s="10">
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30.75">
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
@@ -1329,39 +1484,39 @@
         <v>19</v>
       </c>
       <c r="C20" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>27</v>
-      </c>
       <c r="E20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G20" s="10">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30">
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>29</v>
-      </c>
       <c r="E21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G21" s="10">
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="45">
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6</v>
       </c>
@@ -1369,19 +1524,19 @@
         <v>21</v>
       </c>
       <c r="C22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>31</v>
-      </c>
       <c r="E22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G22" s="10">
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="60">
+    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6</v>
       </c>
@@ -1389,72 +1544,80 @@
         <v>22</v>
       </c>
       <c r="C23" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>33</v>
-      </c>
       <c r="E23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G23" s="10">
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6</v>
       </c>
       <c r="B24">
         <v>23</v>
       </c>
+      <c r="C24" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="D24" s="9" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="E24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G24" s="10">
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
+      <c r="C25" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="D25" s="9" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G25" s="10">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>6</v>
       </c>
       <c r="B26" s="12">
         <v>25</v>
       </c>
-      <c r="C26" s="25"/>
+      <c r="C26" s="13" t="s">
+        <v>86</v>
+      </c>
       <c r="D26" s="14" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F26" s="12"/>
       <c r="G26" s="15">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="75">
+    <row r="27" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>6</v>
       </c>
@@ -1462,74 +1625,80 @@
         <v>26</v>
       </c>
       <c r="C27" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="E27" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="7">
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="45.75">
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6</v>
       </c>
       <c r="B28">
         <v>27</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>38</v>
-      </c>
       <c r="E28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G28" s="10">
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="45.75">
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6</v>
       </c>
       <c r="B29">
         <v>28</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="31" t="s">
-        <v>40</v>
-      </c>
       <c r="E29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G29" s="10">
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6</v>
       </c>
       <c r="B30">
         <v>29</v>
       </c>
+      <c r="C30" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>71</v>
+      </c>
       <c r="E30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G30" s="10">
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>6</v>
       </c>
@@ -1537,20 +1706,20 @@
         <v>30</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="15">
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="76.5">
+    <row r="32" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>6</v>
       </c>
@@ -1558,40 +1727,40 @@
         <v>31</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="E32" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G32" s="10">
         <v>400</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>6</v>
       </c>
       <c r="B33" s="12">
         <v>32</v>
       </c>
-      <c r="C33" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>41</v>
+      <c r="C33" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="15">
         <v>400</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="6"/>
       <c r="C34" s="16"/>
@@ -1606,14 +1775,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
@@ -1622,43 +1791,43 @@
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="90">
-      <c r="A2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="B3">
         <v>50</v>
@@ -1679,56 +1848,56 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="9" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" ht="34.5" customHeight="1">
-      <c r="B6" s="18" t="s">
+      <c r="G6" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="J6" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="19" t="s">
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="18" t="s">
         <v>56</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="18" t="s">
-        <v>60</v>
       </c>
       <c r="C7" s="20">
         <v>100</v>
@@ -1756,9 +1925,9 @@
         <v>950</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C8" s="20">
         <v>100</v>

</xml_diff>